<commit_message>
begin record for parallel Coordinates plot
</commit_message>
<xml_diff>
--- a/records/train_paras.xlsx
+++ b/records/train_paras.xlsx
@@ -397,7 +397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -565,6 +565,44 @@
         <v>0.001</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>my_convnext</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>512</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.3e-05</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>AdamW</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>cosine_warm</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>40</v>
+      </c>
+      <c r="J5" t="n">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="4294967293" verticalDpi="0"/>

</xml_diff>